<commit_message>
El teclado ya reconoce cada tecla
Lo proximo seria integrar el tecladito que esta en Logica con el menu que esta en actualizacion troqueladora. Va queriendo...
</commit_message>
<xml_diff>
--- a/Pines GPIO.xlsx
+++ b/Pines GPIO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t xml:space="preserve">Los siguientes pines son aptos para usar como GPIO porque no tienen ningun periferico colgado </t>
   </si>
@@ -259,6 +259,12 @@
   </si>
   <si>
     <t>E</t>
+  </si>
+  <si>
+    <t>exti</t>
+  </si>
+  <si>
+    <t>out pp</t>
   </si>
 </sst>
 </file>
@@ -410,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -421,27 +427,28 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -722,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,28 +929,28 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8" t="s">
+      <c r="B16" s="15"/>
+      <c r="C16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8" t="s">
+      <c r="D16" s="15"/>
+      <c r="E16" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9" t="s">
+      <c r="F16" s="15"/>
+      <c r="G16" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="12"/>
-      <c r="I16" s="15" t="s">
+      <c r="H16" s="17"/>
+      <c r="I16" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J16" s="19"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -962,20 +969,23 @@
       <c r="F17" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="H17" s="13" t="s">
+      <c r="H17" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="I17" s="10">
+      <c r="I17" s="8">
         <v>1</v>
       </c>
-      <c r="J17" s="17" t="s">
+      <c r="J17" s="12" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K17" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -994,20 +1004,23 @@
       <c r="F18" t="s">
         <v>44</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="H18" s="13" t="s">
+      <c r="H18" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="10">
+      <c r="I18" s="8">
         <v>2</v>
       </c>
-      <c r="J18" s="17" t="s">
+      <c r="J18" s="12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K18" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1020,81 +1033,99 @@
       <c r="D19" t="s">
         <v>61</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="I19" s="10">
+      <c r="I19" s="8">
         <v>3</v>
       </c>
-      <c r="J19" s="17" t="s">
+      <c r="J19" s="12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K19" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>58</v>
       </c>
       <c r="D20" t="s">
         <v>62</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="H20" s="13" t="s">
+      <c r="H20" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="8">
         <v>4</v>
       </c>
-      <c r="J20" s="17" t="s">
+      <c r="J20" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="G21" s="10" t="s">
+      <c r="K20" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G21" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="8">
         <v>5</v>
       </c>
-      <c r="J21" s="17" t="s">
+      <c r="J21" s="12" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G22" s="11" t="s">
+      <c r="K21" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G22" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="H22" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="8">
         <v>6</v>
       </c>
-      <c r="J22" s="17" t="s">
+      <c r="J22" s="12" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="I23" s="10">
+      <c r="K22" s="14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="8">
         <v>7</v>
       </c>
-      <c r="J23" s="17" t="s">
+      <c r="J23" s="12" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="I24" s="11">
+      <c r="K23" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="9">
         <v>8</v>
       </c>
-      <c r="J24" s="18" t="s">
+      <c r="J24" s="13" t="s">
         <v>39</v>
+      </c>
+      <c r="K24" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hay que invertir la logica de las interrupciones
Para poder ponerle las pullup que son la que va. Los sensores andan piola con la logica inversa y un pullup. Las interrupciones si las configuras directo desde el cube andan bien, algo hay oculto.
</commit_message>
<xml_diff>
--- a/Pines GPIO.xlsx
+++ b/Pines GPIO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="83">
   <si>
     <t xml:space="preserve">Los siguientes pines son aptos para usar como GPIO porque no tienen ningun periferico colgado </t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>out pp</t>
+  </si>
+  <si>
+    <t>Sensores</t>
   </si>
 </sst>
 </file>
@@ -286,7 +289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -320,6 +323,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -449,6 +458,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,17 +742,17 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -759,7 +769,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -776,7 +786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
@@ -789,12 +799,12 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="20" t="s">
         <v>41</v>
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>40</v>
       </c>
@@ -807,14 +817,14 @@
       <c r="D5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="20" t="s">
         <v>31</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -834,7 +844,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -854,7 +864,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -867,8 +877,11 @@
       <c r="E8" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="H8" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -882,7 +895,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -896,7 +909,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -907,7 +920,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -918,17 +931,17 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>47</v>
       </c>
@@ -950,7 +963,7 @@
       </c>
       <c r="J16" s="19"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -985,7 +998,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1020,7 +1033,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1049,7 +1062,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="C20" t="s">
         <v>58</v>
       </c>
@@ -1072,7 +1085,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="G21" s="8" t="s">
         <v>78</v>
       </c>
@@ -1089,7 +1102,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="G22" s="9" t="s">
         <v>79</v>
       </c>
@@ -1106,7 +1119,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="I23" s="8">
         <v>7</v>
       </c>
@@ -1117,7 +1130,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="I24" s="9">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Acomodado el cube de "final"
Ya esta todo listo para empezar a programar posta.
</commit_message>
<xml_diff>
--- a/Pines GPIO.xlsx
+++ b/Pines GPIO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="95">
   <si>
     <t xml:space="preserve">Los siguientes pines son aptos para usar como GPIO porque no tienen ningun periferico colgado </t>
   </si>
@@ -274,6 +274,36 @@
   </si>
   <si>
     <t>PA1</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Unidades</t>
+  </si>
+  <si>
+    <t>Golpes</t>
   </si>
 </sst>
 </file>
@@ -295,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +371,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -455,6 +491,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -470,14 +514,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,17 +805,17 @@
   <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -788,7 +832,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -805,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -823,7 +867,7 @@
       </c>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
@@ -843,7 +887,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -863,7 +907,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -886,7 +930,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B8" s="6" t="s">
         <v>3</v>
       </c>
@@ -903,7 +947,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -917,7 +961,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>25</v>
       </c>
@@ -931,7 +975,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -942,7 +986,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -953,39 +997,39 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="15"/>
-      <c r="C16" s="15" t="s">
+      <c r="B16" s="19"/>
+      <c r="C16" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15" t="s">
+      <c r="D16" s="19"/>
+      <c r="E16" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="16" t="s">
+      <c r="F16" s="19"/>
+      <c r="G16" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="17"/>
-      <c r="I16" s="18" t="s">
+      <c r="H16" s="21"/>
+      <c r="I16" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="19"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="23"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -1010,8 +1054,8 @@
       <c r="H17" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="7">
-        <v>1</v>
+      <c r="I17" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="J17" s="11" t="s">
         <v>33</v>
@@ -1020,7 +1064,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1045,8 +1089,8 @@
       <c r="H18" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="7">
-        <v>2</v>
+      <c r="I18" s="7" t="s">
+        <v>90</v>
       </c>
       <c r="J18" s="11" t="s">
         <v>35</v>
@@ -1055,7 +1099,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1068,18 +1112,18 @@
       <c r="D19" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="21"/>
+      <c r="F19" s="18"/>
       <c r="G19" s="7" t="s">
         <v>74</v>
       </c>
       <c r="H19" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="7">
-        <v>3</v>
+      <c r="I19" s="7" t="s">
+        <v>91</v>
       </c>
       <c r="J19" s="11" t="s">
         <v>37</v>
@@ -1088,7 +1132,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="25"/>
       <c r="C20" t="s">
         <v>58</v>
       </c>
@@ -1098,7 +1146,7 @@
       <c r="E20" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="15" t="s">
         <v>83</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -1107,8 +1155,8 @@
       <c r="H20" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="I20" s="7">
-        <v>4</v>
+      <c r="I20" s="7" t="s">
+        <v>92</v>
       </c>
       <c r="J20" s="11" t="s">
         <v>39</v>
@@ -1117,11 +1165,17 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="E21" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="23" t="s">
+      <c r="F21" s="16" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="7" t="s">
@@ -1130,8 +1184,8 @@
       <c r="H21" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="7">
-        <v>5</v>
+      <c r="I21" s="7" t="s">
+        <v>85</v>
       </c>
       <c r="J21" s="11" t="s">
         <v>84</v>
@@ -1140,15 +1194,21 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>26</v>
+      </c>
       <c r="G22" s="8" t="s">
         <v>77</v>
       </c>
       <c r="H22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="7">
-        <v>6</v>
+      <c r="I22" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="J22" s="11" t="s">
         <v>27</v>
@@ -1157,9 +1217,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="I23" s="7">
-        <v>7</v>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="I23" s="7" t="s">
+        <v>87</v>
       </c>
       <c r="J23" s="11" t="s">
         <v>29</v>
@@ -1168,9 +1228,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I24" s="8">
-        <v>8</v>
+    <row r="24" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I24" s="8" t="s">
+        <v>88</v>
       </c>
       <c r="J24" s="12" t="s">
         <v>31</v>
@@ -1183,13 +1243,14 @@
   <sortState ref="A3:A46">
     <sortCondition ref="A3:A46"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="A20:B20"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="E16:F16"/>
     <mergeCell ref="G16:H16"/>
-    <mergeCell ref="I16:J16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Lo mismo de abajo
</commit_message>
<xml_diff>
--- a/Pines GPIO.xlsx
+++ b/Pines GPIO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="110">
   <si>
     <t xml:space="preserve">Los siguientes pines son aptos para usar como GPIO porque no tienen ningun periferico colgado </t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>SDA(GPIO)</t>
+  </si>
+  <si>
+    <t>Uso futuro</t>
   </si>
 </sst>
 </file>
@@ -374,7 +377,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,6 +438,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -552,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -614,6 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -901,21 +911,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="13" max="16" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -932,7 +943,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -949,7 +960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -969,7 +980,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
@@ -989,7 +1000,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1009,7 +1020,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1032,7 +1043,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
@@ -1049,7 +1060,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -1062,22 +1073,25 @@
       <c r="E9" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="H9" s="33" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="33" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="33" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -1088,28 +1102,28 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="33" t="s">
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
         <v>47</v>
       </c>
@@ -1143,7 +1157,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
@@ -1190,7 +1204,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -1237,7 +1251,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
@@ -1282,7 +1296,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>108</v>
       </c>
@@ -1321,7 +1335,7 @@
       </c>
       <c r="O20" s="23"/>
     </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="26" t="s">
         <v>80</v>
       </c>
@@ -1360,7 +1374,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>93</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
         <v>94</v>
       </c>
@@ -1400,7 +1414,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I24" s="7" t="s">
         <v>88</v>
       </c>

</xml_diff>

<commit_message>
Avances de informe final
</commit_message>
<xml_diff>
--- a/Pines GPIO.xlsx
+++ b/Pines GPIO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="162">
   <si>
     <t xml:space="preserve">Los siguientes pines son aptos para usar como GPIO porque no tienen ningun periferico colgado </t>
   </si>
@@ -406,6 +406,105 @@
   </si>
   <si>
     <t>…</t>
+  </si>
+  <si>
+    <t>RFID_MOSI</t>
+  </si>
+  <si>
+    <t>SPI1_MOSI</t>
+  </si>
+  <si>
+    <t>RFID_MISO</t>
+  </si>
+  <si>
+    <t>SPI1_MISO</t>
+  </si>
+  <si>
+    <t>RFID_SCK</t>
+  </si>
+  <si>
+    <t>SPI1_SCK</t>
+  </si>
+  <si>
+    <t>Denominación</t>
+  </si>
+  <si>
+    <t>Modo</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Teclado F1</t>
+  </si>
+  <si>
+    <t>Input mode</t>
+  </si>
+  <si>
+    <t>Teclado F2</t>
+  </si>
+  <si>
+    <t>Teclado F3</t>
+  </si>
+  <si>
+    <t>Teclado F4</t>
+  </si>
+  <si>
+    <t>Teclado C1</t>
+  </si>
+  <si>
+    <t>Output Push Pull</t>
+  </si>
+  <si>
+    <t>Sensor unidades</t>
+  </si>
+  <si>
+    <t>External Interrupt Mode with Rising edge trigger detection</t>
+  </si>
+  <si>
+    <t>Led Azul</t>
+  </si>
+  <si>
+    <t>Led Rojo</t>
+  </si>
+  <si>
+    <t>Led Naranja</t>
+  </si>
+  <si>
+    <t>Led Verde</t>
+  </si>
+  <si>
+    <t>Display D4</t>
+  </si>
+  <si>
+    <t>Display D5</t>
+  </si>
+  <si>
+    <t>Display D6</t>
+  </si>
+  <si>
+    <t>Display D7</t>
+  </si>
+  <si>
+    <t>Teclado C3</t>
+  </si>
+  <si>
+    <t>Sensor golpes</t>
+  </si>
+  <si>
+    <t>Display RS</t>
+  </si>
+  <si>
+    <t>Display E</t>
+  </si>
+  <si>
+    <t>Teclado C2</t>
+  </si>
+  <si>
+    <t>RFID_SDA</t>
+  </si>
+  <si>
+    <t>Teclado C4</t>
   </si>
 </sst>
 </file>
@@ -526,7 +625,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -847,11 +946,69 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,87 +1044,117 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1255,8 +1442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A81" sqref="A81"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q45" sqref="Q45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1469,26 +1656,26 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A16" s="32" t="s">
+      <c r="A16" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="34" t="s">
+      <c r="B16" s="48"/>
+      <c r="C16" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34" t="s">
+      <c r="D16" s="49"/>
+      <c r="E16" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="34"/>
-      <c r="G16" s="35" t="s">
+      <c r="F16" s="49"/>
+      <c r="G16" s="50" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="36"/>
-      <c r="I16" s="28" t="s">
+      <c r="H16" s="51"/>
+      <c r="I16" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="29"/>
+      <c r="J16" s="44"/>
       <c r="M16" s="18">
         <v>1</v>
       </c>
@@ -1609,10 +1796,10 @@
       <c r="D19" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="47" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="33"/>
+      <c r="F19" s="48"/>
       <c r="G19" s="6" t="s">
         <v>74</v>
       </c>
@@ -1675,20 +1862,20 @@
       <c r="K20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="N20" s="27" t="s">
+      <c r="N20" s="42" t="s">
         <v>101</v>
       </c>
-      <c r="O20" s="27"/>
+      <c r="O20" s="42"/>
     </row>
     <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="30" t="s">
+      <c r="A21" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="37" t="s">
+      <c r="B21" s="46"/>
+      <c r="C21" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="D21" s="38"/>
+      <c r="D21" s="53"/>
       <c r="E21" s="24" t="s">
         <v>68</v>
       </c>
@@ -1787,760 +1974,994 @@
       </c>
     </row>
     <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="34"/>
-      <c r="E29" s="34" t="s">
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="F29" s="34"/>
-      <c r="G29" s="34"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
     </row>
     <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B30" s="40" t="s">
+      <c r="B30" s="54" t="s">
         <v>118</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="42" t="s">
+      <c r="C30" s="55"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="F30" s="43" t="s">
+      <c r="F30" s="29" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A31" s="44">
+      <c r="A31" s="30">
         <v>0</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="46"/>
-      <c r="D31" s="46"/>
-      <c r="E31" s="47">
+      <c r="C31" s="57"/>
+      <c r="D31" s="57"/>
+      <c r="E31" s="31">
         <v>2</v>
       </c>
-      <c r="F31" s="48">
+      <c r="F31" s="32">
         <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A32" s="49">
+      <c r="A32" s="33">
         <f>A31+E31</f>
         <v>2</v>
       </c>
-      <c r="B32" s="50" t="s">
+      <c r="B32" s="58" t="s">
         <v>122</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="52">
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="34">
         <v>9</v>
       </c>
-      <c r="F32" s="53">
+      <c r="F32" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="49">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A33" s="33">
         <f t="shared" ref="A33:A44" si="0">A32+E32</f>
         <v>11</v>
       </c>
-      <c r="B33" s="50" t="s">
+      <c r="B33" s="58" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="52">
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="34">
         <v>5</v>
       </c>
-      <c r="F33" s="53">
+      <c r="F33" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="49">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A34" s="33">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B34" s="50" t="s">
+      <c r="B34" s="58" t="s">
         <v>124</v>
       </c>
-      <c r="C34" s="51"/>
-      <c r="D34" s="51"/>
-      <c r="E34" s="52">
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="34">
         <v>4</v>
       </c>
-      <c r="F34" s="53">
+      <c r="F34" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="49">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A35" s="33">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B35" s="50" t="s">
+      <c r="B35" s="58" t="s">
         <v>125</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52">
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="34">
         <v>4</v>
       </c>
-      <c r="F35" s="53">
+      <c r="F35" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="49">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A36" s="33">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B36" s="50" t="s">
+      <c r="B36" s="58" t="s">
         <v>126</v>
       </c>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="52">
+      <c r="C36" s="59"/>
+      <c r="D36" s="59"/>
+      <c r="E36" s="34">
         <v>2</v>
       </c>
-      <c r="F36" s="53">
+      <c r="F36" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="49">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A37" s="33">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B37" s="54" t="s">
+      <c r="B37" s="64" t="s">
         <v>109</v>
       </c>
-      <c r="C37" s="55"/>
-      <c r="D37" s="55"/>
-      <c r="E37" s="52">
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="34">
         <v>6</v>
       </c>
-      <c r="F37" s="53">
+      <c r="F37" s="35">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" s="56">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A38" s="36">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="60" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="58"/>
-      <c r="D38" s="58"/>
-      <c r="E38" s="59">
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="37">
         <v>2</v>
       </c>
-      <c r="F38" s="60">
+      <c r="F38" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" s="56">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A39" s="36">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B39" s="57" t="s">
+      <c r="B39" s="60" t="s">
         <v>122</v>
       </c>
-      <c r="C39" s="58"/>
-      <c r="D39" s="58"/>
-      <c r="E39" s="59">
+      <c r="C39" s="61"/>
+      <c r="D39" s="61"/>
+      <c r="E39" s="37">
         <v>10</v>
       </c>
-      <c r="F39" s="60">
+      <c r="F39" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="56">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A40" s="36">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B40" s="57" t="s">
+      <c r="B40" s="60" t="s">
         <v>123</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="59">
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="37">
         <v>6</v>
       </c>
-      <c r="F40" s="60">
+      <c r="F40" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" s="56">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A41" s="36">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B41" s="57" t="s">
+      <c r="B41" s="60" t="s">
         <v>124</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="59">
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="37">
         <v>4</v>
       </c>
-      <c r="F41" s="60">
+      <c r="F41" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A42" s="56">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A42" s="36">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B42" s="57" t="s">
+      <c r="B42" s="60" t="s">
         <v>125</v>
       </c>
-      <c r="C42" s="58"/>
-      <c r="D42" s="58"/>
-      <c r="E42" s="59">
+      <c r="C42" s="61"/>
+      <c r="D42" s="61"/>
+      <c r="E42" s="37">
         <v>4</v>
       </c>
-      <c r="F42" s="60">
+      <c r="F42" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A43" s="56">
+    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="36">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B43" s="57" t="s">
+      <c r="B43" s="60" t="s">
         <v>126</v>
       </c>
-      <c r="C43" s="58"/>
-      <c r="D43" s="58"/>
-      <c r="E43" s="59">
+      <c r="C43" s="61"/>
+      <c r="D43" s="61"/>
+      <c r="E43" s="37">
         <v>2</v>
       </c>
-      <c r="F43" s="60">
+      <c r="F43" s="38">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A44" s="56">
+    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="36">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B44" s="61" t="s">
+      <c r="B44" s="62" t="s">
         <v>109</v>
       </c>
-      <c r="C44" s="62"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="59">
+      <c r="C44" s="63"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="37">
         <v>6</v>
       </c>
-      <c r="F44" s="60">
+      <c r="F44" s="38">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A45" s="49">
+      <c r="L44" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="M44" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="N44" s="77" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="33">
         <v>64</v>
       </c>
-      <c r="B45" s="50" t="s">
+      <c r="B45" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C45" s="51"/>
-      <c r="D45" s="51"/>
-      <c r="E45" s="52">
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="34">
         <v>2</v>
       </c>
-      <c r="F45" s="53">
+      <c r="F45" s="35">
         <v>2</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A46" s="49"/>
-      <c r="B46" s="54" t="s">
+      <c r="L45" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="M45" s="75" t="s">
+        <v>144</v>
+      </c>
+      <c r="N45" s="74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="33"/>
+      <c r="B46" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C46" s="55"/>
-      <c r="D46" s="55"/>
-      <c r="E46" s="52"/>
-      <c r="F46" s="53"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" s="56">
+      <c r="C46" s="65"/>
+      <c r="D46" s="65"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="35"/>
+      <c r="L46" s="73" t="s">
+        <v>107</v>
+      </c>
+      <c r="M46" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N46" s="71" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="36">
         <f>A45+32</f>
         <v>96</v>
       </c>
-      <c r="B47" s="57" t="s">
+      <c r="B47" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
-      <c r="E47" s="59">
+      <c r="C47" s="61"/>
+      <c r="D47" s="61"/>
+      <c r="E47" s="37">
         <v>2</v>
       </c>
-      <c r="F47" s="60">
+      <c r="F47" s="38">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" s="56"/>
-      <c r="B48" s="61" t="s">
+      <c r="L47" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="M47" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N47" s="71" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="36"/>
+      <c r="B48" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C48" s="62"/>
-      <c r="D48" s="62"/>
-      <c r="E48" s="59"/>
-      <c r="F48" s="60"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" s="49">
+      <c r="C48" s="63"/>
+      <c r="D48" s="63"/>
+      <c r="E48" s="37"/>
+      <c r="F48" s="38"/>
+      <c r="L48" s="73" t="s">
+        <v>4</v>
+      </c>
+      <c r="M48" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N48" s="71" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="33">
         <f>A47+32</f>
         <v>128</v>
       </c>
-      <c r="B49" s="50" t="s">
+      <c r="B49" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C49" s="51"/>
-      <c r="D49" s="51"/>
-      <c r="E49" s="52">
+      <c r="C49" s="59"/>
+      <c r="D49" s="59"/>
+      <c r="E49" s="34">
         <v>2</v>
       </c>
-      <c r="F49" s="53">
+      <c r="F49" s="35">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" s="49"/>
-      <c r="B50" s="54" t="s">
+      <c r="L49" s="73" t="s">
+        <v>3</v>
+      </c>
+      <c r="M49" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N49" s="71" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="33"/>
+      <c r="B50" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C50" s="55"/>
-      <c r="D50" s="55"/>
-      <c r="E50" s="52"/>
-      <c r="F50" s="53"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="56">
+      <c r="C50" s="65"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="35"/>
+      <c r="L50" s="73" t="s">
+        <v>26</v>
+      </c>
+      <c r="M50" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N50" s="71" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="36">
         <f>A49+32</f>
         <v>160</v>
       </c>
-      <c r="B51" s="57" t="s">
+      <c r="B51" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
-      <c r="E51" s="59">
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="37">
         <v>2</v>
       </c>
-      <c r="F51" s="60">
+      <c r="F51" s="38">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A52" s="56"/>
-      <c r="B52" s="61" t="s">
+      <c r="L51" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="M51" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N51" s="71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="36"/>
+      <c r="B52" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C52" s="62"/>
-      <c r="D52" s="62"/>
-      <c r="E52" s="59"/>
-      <c r="F52" s="60"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="49">
+      <c r="C52" s="63"/>
+      <c r="D52" s="63"/>
+      <c r="E52" s="37"/>
+      <c r="F52" s="38"/>
+      <c r="L52" s="73" t="s">
+        <v>13</v>
+      </c>
+      <c r="M52" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N52" s="71" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="33">
         <f>A51+32</f>
         <v>192</v>
       </c>
-      <c r="B53" s="50" t="s">
+      <c r="B53" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="52">
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="34">
         <v>2</v>
       </c>
-      <c r="F53" s="53">
+      <c r="F53" s="35">
         <v>6</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A54" s="49"/>
-      <c r="B54" s="54" t="s">
+      <c r="L53" s="73" t="s">
+        <v>12</v>
+      </c>
+      <c r="M53" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N53" s="71" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="33"/>
+      <c r="B54" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C54" s="55"/>
-      <c r="D54" s="55"/>
-      <c r="E54" s="52"/>
-      <c r="F54" s="53"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" s="56">
+      <c r="C54" s="65"/>
+      <c r="D54" s="65"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="35"/>
+      <c r="L54" s="73" t="s">
+        <v>9</v>
+      </c>
+      <c r="M54" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N54" s="71" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="36">
         <f>A53+32</f>
         <v>224</v>
       </c>
-      <c r="B55" s="57" t="s">
+      <c r="B55" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C55" s="58"/>
-      <c r="D55" s="58"/>
-      <c r="E55" s="59">
+      <c r="C55" s="61"/>
+      <c r="D55" s="61"/>
+      <c r="E55" s="37">
         <v>2</v>
       </c>
-      <c r="F55" s="60">
+      <c r="F55" s="38">
         <v>7</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="56"/>
-      <c r="B56" s="61" t="s">
+      <c r="L55" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="M55" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N55" s="71" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="36"/>
+      <c r="B56" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="59"/>
-      <c r="F56" s="60"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A57" s="49">
+      <c r="C56" s="63"/>
+      <c r="D56" s="63"/>
+      <c r="E56" s="37"/>
+      <c r="F56" s="38"/>
+      <c r="L56" s="73" t="s">
+        <v>62</v>
+      </c>
+      <c r="M56" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N56" s="71" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="33">
         <f>A55+32</f>
         <v>256</v>
       </c>
-      <c r="B57" s="50" t="s">
+      <c r="B57" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="52">
+      <c r="C57" s="59"/>
+      <c r="D57" s="59"/>
+      <c r="E57" s="34">
         <v>2</v>
       </c>
-      <c r="F57" s="53">
+      <c r="F57" s="35">
         <v>8</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A58" s="49"/>
-      <c r="B58" s="54" t="s">
+      <c r="L57" s="73" t="s">
+        <v>61</v>
+      </c>
+      <c r="M57" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N57" s="71" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="33"/>
+      <c r="B58" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C58" s="55"/>
-      <c r="D58" s="55"/>
-      <c r="E58" s="52"/>
-      <c r="F58" s="53"/>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A59" s="56">
+      <c r="C58" s="65"/>
+      <c r="D58" s="65"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="35"/>
+      <c r="L58" s="73" t="s">
+        <v>60</v>
+      </c>
+      <c r="M58" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N58" s="71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="36">
         <f>A57+32</f>
         <v>288</v>
       </c>
-      <c r="B59" s="57" t="s">
+      <c r="B59" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C59" s="58"/>
-      <c r="D59" s="58"/>
-      <c r="E59" s="59">
+      <c r="C59" s="61"/>
+      <c r="D59" s="61"/>
+      <c r="E59" s="37">
         <v>2</v>
       </c>
-      <c r="F59" s="60">
+      <c r="F59" s="38">
         <v>9</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" s="56"/>
-      <c r="B60" s="61" t="s">
+      <c r="L59" s="73" t="s">
+        <v>59</v>
+      </c>
+      <c r="M59" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N59" s="71" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A60" s="36"/>
+      <c r="B60" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C60" s="62"/>
-      <c r="D60" s="62"/>
-      <c r="E60" s="59"/>
-      <c r="F60" s="60"/>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="49">
+      <c r="C60" s="63"/>
+      <c r="D60" s="63"/>
+      <c r="E60" s="37"/>
+      <c r="F60" s="38"/>
+      <c r="L60" s="73" t="s">
+        <v>41</v>
+      </c>
+      <c r="M60" s="72" t="s">
+        <v>146</v>
+      </c>
+      <c r="N60" s="71" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="33">
         <f>A59+32</f>
         <v>320</v>
       </c>
-      <c r="B61" s="50" t="s">
+      <c r="B61" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C61" s="51"/>
-      <c r="D61" s="51"/>
-      <c r="E61" s="52">
+      <c r="C61" s="59"/>
+      <c r="D61" s="59"/>
+      <c r="E61" s="34">
         <v>2</v>
       </c>
-      <c r="F61" s="53">
+      <c r="F61" s="35">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A62" s="49"/>
-      <c r="B62" s="54" t="s">
+      <c r="L61" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="M61" s="72" t="s">
+        <v>144</v>
+      </c>
+      <c r="N61" s="71" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="33"/>
+      <c r="B62" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C62" s="55"/>
-      <c r="D62" s="55"/>
-      <c r="E62" s="52"/>
-      <c r="F62" s="53"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="56">
+      <c r="C62" s="65"/>
+      <c r="D62" s="65"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="35"/>
+      <c r="L62" s="73" t="s">
+        <v>33</v>
+      </c>
+      <c r="M62" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="N62" s="71" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A63" s="36">
         <f>A61+32</f>
         <v>352</v>
       </c>
-      <c r="B63" s="57" t="s">
+      <c r="B63" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C63" s="58"/>
-      <c r="D63" s="58"/>
-      <c r="E63" s="59">
+      <c r="C63" s="61"/>
+      <c r="D63" s="61"/>
+      <c r="E63" s="37">
         <v>2</v>
       </c>
-      <c r="F63" s="60">
+      <c r="F63" s="38">
         <v>11</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A64" s="56"/>
-      <c r="B64" s="61" t="s">
+      <c r="L63" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="M63" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="N63" s="71" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A64" s="36"/>
+      <c r="B64" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C64" s="62"/>
-      <c r="D64" s="62"/>
-      <c r="E64" s="59"/>
-      <c r="F64" s="60"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" s="49">
+      <c r="C64" s="63"/>
+      <c r="D64" s="63"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="38"/>
+      <c r="L64" s="73" t="s">
+        <v>37</v>
+      </c>
+      <c r="M64" s="72" t="s">
+        <v>139</v>
+      </c>
+      <c r="N64" s="71" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="33">
         <f>A63+32</f>
         <v>384</v>
       </c>
-      <c r="B65" s="50" t="s">
+      <c r="B65" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="52">
+      <c r="C65" s="59"/>
+      <c r="D65" s="59"/>
+      <c r="E65" s="34">
         <v>2</v>
       </c>
-      <c r="F65" s="53">
+      <c r="F65" s="35">
         <v>12</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="49"/>
-      <c r="B66" s="54" t="s">
+      <c r="L65" s="70" t="s">
+        <v>39</v>
+      </c>
+      <c r="M65" s="69" t="s">
+        <v>139</v>
+      </c>
+      <c r="N65" s="68" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="33"/>
+      <c r="B66" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C66" s="55"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="53"/>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" s="56">
+      <c r="C66" s="65"/>
+      <c r="D66" s="65"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="35"/>
+    </row>
+    <row r="67" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="36">
         <f>A65+32</f>
         <v>416</v>
       </c>
-      <c r="B67" s="57" t="s">
+      <c r="B67" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C67" s="58"/>
-      <c r="D67" s="58"/>
-      <c r="E67" s="59">
+      <c r="C67" s="61"/>
+      <c r="D67" s="61"/>
+      <c r="E67" s="37">
         <v>2</v>
       </c>
-      <c r="F67" s="60">
+      <c r="F67" s="38">
         <v>13</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="56"/>
-      <c r="B68" s="61" t="s">
+      <c r="L67" s="79" t="s">
+        <v>137</v>
+      </c>
+      <c r="M67" s="78" t="s">
+        <v>136</v>
+      </c>
+      <c r="N67" s="77" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A68" s="36"/>
+      <c r="B68" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C68" s="62"/>
-      <c r="D68" s="62"/>
-      <c r="E68" s="59"/>
-      <c r="F68" s="60"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="49">
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="38"/>
+      <c r="L68" s="76" t="s">
+        <v>49</v>
+      </c>
+      <c r="M68" s="75" t="s">
+        <v>134</v>
+      </c>
+      <c r="N68" s="74" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A69" s="33">
         <f>A67+32</f>
         <v>448</v>
       </c>
-      <c r="B69" s="50" t="s">
+      <c r="B69" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C69" s="51"/>
-      <c r="D69" s="51"/>
-      <c r="E69" s="52">
+      <c r="C69" s="59"/>
+      <c r="D69" s="59"/>
+      <c r="E69" s="34">
         <v>2</v>
       </c>
-      <c r="F69" s="53">
+      <c r="F69" s="35">
         <v>14</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="49"/>
-      <c r="B70" s="54" t="s">
+      <c r="L69" s="73" t="s">
+        <v>51</v>
+      </c>
+      <c r="M69" s="72" t="s">
+        <v>132</v>
+      </c>
+      <c r="N69" s="71" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="33"/>
+      <c r="B70" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C70" s="55"/>
-      <c r="D70" s="55"/>
-      <c r="E70" s="52"/>
-      <c r="F70" s="53"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="56">
+      <c r="C70" s="65"/>
+      <c r="D70" s="65"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="35"/>
+      <c r="L70" s="70" t="s">
+        <v>53</v>
+      </c>
+      <c r="M70" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="N70" s="68" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A71" s="36">
         <f>A69+32</f>
         <v>480</v>
       </c>
-      <c r="B71" s="57" t="s">
+      <c r="B71" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C71" s="58"/>
-      <c r="D71" s="58"/>
-      <c r="E71" s="59">
+      <c r="C71" s="61"/>
+      <c r="D71" s="61"/>
+      <c r="E71" s="37">
         <v>2</v>
       </c>
-      <c r="F71" s="60">
+      <c r="F71" s="38">
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A72" s="56"/>
-      <c r="B72" s="61" t="s">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A72" s="36"/>
+      <c r="B72" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C72" s="62"/>
-      <c r="D72" s="62"/>
-      <c r="E72" s="59"/>
-      <c r="F72" s="60"/>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A73" s="49">
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="38"/>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A73" s="33">
         <f>A71+32</f>
         <v>512</v>
       </c>
-      <c r="B73" s="50" t="s">
+      <c r="B73" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C73" s="51"/>
-      <c r="D73" s="51"/>
-      <c r="E73" s="52">
+      <c r="C73" s="59"/>
+      <c r="D73" s="59"/>
+      <c r="E73" s="34">
         <v>2</v>
       </c>
-      <c r="F73" s="53">
+      <c r="F73" s="35">
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="49"/>
-      <c r="B74" s="54" t="s">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A74" s="33"/>
+      <c r="B74" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C74" s="55"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="52"/>
-      <c r="F74" s="53"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="56">
+      <c r="C74" s="65"/>
+      <c r="D74" s="65"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="35"/>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A75" s="36">
         <f>A73+32</f>
         <v>544</v>
       </c>
-      <c r="B75" s="57" t="s">
+      <c r="B75" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C75" s="58"/>
-      <c r="D75" s="58"/>
-      <c r="E75" s="59">
+      <c r="C75" s="61"/>
+      <c r="D75" s="61"/>
+      <c r="E75" s="37">
         <v>2</v>
       </c>
-      <c r="F75" s="60">
+      <c r="F75" s="38">
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="56"/>
-      <c r="B76" s="61" t="s">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A76" s="36"/>
+      <c r="B76" s="62" t="s">
         <v>128</v>
       </c>
-      <c r="C76" s="62"/>
-      <c r="D76" s="62"/>
-      <c r="E76" s="59"/>
-      <c r="F76" s="60"/>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A77" s="49">
+      <c r="C76" s="63"/>
+      <c r="D76" s="63"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="38"/>
+    </row>
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A77" s="33">
         <f>A75+32</f>
         <v>576</v>
       </c>
-      <c r="B77" s="50" t="s">
+      <c r="B77" s="58" t="s">
         <v>127</v>
       </c>
-      <c r="C77" s="51"/>
-      <c r="D77" s="51"/>
-      <c r="E77" s="52">
+      <c r="C77" s="59"/>
+      <c r="D77" s="59"/>
+      <c r="E77" s="34">
         <v>2</v>
       </c>
-      <c r="F77" s="53">
+      <c r="F77" s="35">
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A78" s="49"/>
-      <c r="B78" s="54" t="s">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A78" s="33"/>
+      <c r="B78" s="64" t="s">
         <v>128</v>
       </c>
-      <c r="C78" s="55"/>
-      <c r="D78" s="55"/>
-      <c r="E78" s="52"/>
-      <c r="F78" s="53"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" s="56">
+      <c r="C78" s="65"/>
+      <c r="D78" s="65"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="35"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A79" s="36">
         <f>A77+32</f>
         <v>608</v>
       </c>
-      <c r="B79" s="57" t="s">
+      <c r="B79" s="60" t="s">
         <v>127</v>
       </c>
-      <c r="C79" s="58"/>
-      <c r="D79" s="58"/>
-      <c r="E79" s="59">
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="37">
         <v>2</v>
       </c>
-      <c r="F79" s="60">
+      <c r="F79" s="38">
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A80" s="63">
+    <row r="80" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="39">
         <f>A79+26</f>
         <v>634</v>
       </c>
-      <c r="B80" s="64" t="s">
+      <c r="B80" s="66" t="s">
         <v>109</v>
       </c>
-      <c r="C80" s="65"/>
-      <c r="D80" s="65"/>
-      <c r="E80" s="66">
+      <c r="C80" s="67"/>
+      <c r="D80" s="67"/>
+      <c r="E80" s="40">
         <v>6</v>
       </c>
-      <c r="F80" s="67">
+      <c r="F80" s="41">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Agregado de display secundario y boton de descuento
Se agrega comunicación UART para repetir la indicación de unidades en un display secundario más grande para facilitar la visión del operario. Además se agrega un botón que permite descontar una unidad por si la misma salió mal troquelada.
</commit_message>
<xml_diff>
--- a/Pines GPIO.xlsx
+++ b/Pines GPIO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="180">
   <si>
     <t xml:space="preserve">Los siguientes pines son aptos para usar como GPIO porque no tienen ningun periferico colgado </t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>0x45</t>
+  </si>
+  <si>
+    <t>Input (tienen pull up externo)</t>
   </si>
 </sst>
 </file>
@@ -1143,6 +1146,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1207,15 +1219,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2470,23 +2473,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="K90" sqref="K90"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="5.7109375" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>63</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>45</v>
       </c>
@@ -2520,7 +2523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>44</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>40</v>
       </c>
@@ -2560,7 +2563,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2580,7 +2583,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2603,7 +2606,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
@@ -2620,7 +2623,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -2636,8 +2639,11 @@
       <c r="H9" s="23" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B10" s="23" t="s">
         <v>25</v>
       </c>
@@ -2651,7 +2657,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>24</v>
       </c>
@@ -2662,7 +2668,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>23</v>
       </c>
@@ -2673,43 +2679,43 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="E13" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="60" t="s">
+    <row r="16" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="63" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="61"/>
-      <c r="C16" s="62" t="s">
+      <c r="B16" s="64"/>
+      <c r="C16" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="62"/>
-      <c r="E16" s="62" t="s">
+      <c r="D16" s="65"/>
+      <c r="E16" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="F16" s="62"/>
-      <c r="G16" s="63" t="s">
+      <c r="F16" s="65"/>
+      <c r="G16" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="H16" s="64"/>
-      <c r="I16" s="56" t="s">
+      <c r="H16" s="67"/>
+      <c r="I16" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="J16" s="57"/>
+      <c r="J16" s="60"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
       <c r="P16" s="19"/>
     </row>
-    <row r="17" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
@@ -2748,7 +2754,7 @@
       <c r="O17" s="18"/>
       <c r="P17" s="19"/>
     </row>
-    <row r="18" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>50</v>
       </c>
@@ -2787,7 +2793,7 @@
       <c r="O18" s="18"/>
       <c r="P18" s="19"/>
     </row>
-    <row r="19" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
         <v>52</v>
       </c>
@@ -2800,10 +2806,10 @@
       <c r="D19" t="s">
         <v>61</v>
       </c>
-      <c r="E19" s="60" t="s">
+      <c r="E19" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="61"/>
+      <c r="F19" s="64"/>
       <c r="G19" s="6" t="s">
         <v>74</v>
       </c>
@@ -2828,7 +2834,7 @@
       </c>
       <c r="P19" s="19"/>
     </row>
-    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="7" t="s">
         <v>102</v>
       </c>
@@ -2862,20 +2868,20 @@
       <c r="K20" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="N20" s="55" t="s">
+      <c r="N20" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="O20" s="55"/>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
+      <c r="O20" s="58"/>
+    </row>
+    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="59"/>
-      <c r="C21" s="65" t="s">
+      <c r="B21" s="62"/>
+      <c r="C21" s="68" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="66"/>
+      <c r="D21" s="69"/>
       <c r="E21" s="24" t="s">
         <v>68</v>
       </c>
@@ -2910,7 +2916,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>93</v>
       </c>
@@ -2939,7 +2945,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="7" t="s">
         <v>94</v>
       </c>
@@ -2962,7 +2968,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I24" s="7" t="s">
         <v>88</v>
       </c>
@@ -2973,28 +2979,28 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="62" t="s">
+    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="65" t="s">
         <v>109</v>
       </c>
-      <c r="B29" s="62"/>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62" t="s">
+      <c r="B29" s="65"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65" t="s">
         <v>110</v>
       </c>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-    </row>
-    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F29" s="65"/>
+      <c r="G29" s="65"/>
+    </row>
+    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="67" t="s">
+      <c r="B30" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="68"/>
-      <c r="D30" s="68"/>
+      <c r="C30" s="71"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="28" t="s">
         <v>113</v>
       </c>
@@ -3002,15 +3008,15 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A31" s="30">
         <v>0</v>
       </c>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="72" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="70"/>
-      <c r="D31" s="70"/>
+      <c r="C31" s="73"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="31">
         <v>2</v>
       </c>
@@ -3018,16 +3024,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A32" s="33">
         <f>A31+E31</f>
         <v>2</v>
       </c>
-      <c r="B32" s="71" t="s">
+      <c r="B32" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="C32" s="72"/>
-      <c r="D32" s="72"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
       <c r="E32" s="34">
         <v>9</v>
       </c>
@@ -3035,16 +3041,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="33">
         <f t="shared" ref="A33:A44" si="0">A32+E32</f>
         <v>11</v>
       </c>
-      <c r="B33" s="71" t="s">
+      <c r="B33" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="C33" s="72"/>
-      <c r="D33" s="72"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
       <c r="E33" s="34">
         <v>5</v>
       </c>
@@ -3052,16 +3058,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="33">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B34" s="71" t="s">
+      <c r="B34" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="72"/>
-      <c r="D34" s="72"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
       <c r="E34" s="34">
         <v>4</v>
       </c>
@@ -3069,16 +3075,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="33">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B35" s="71" t="s">
+      <c r="B35" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="72"/>
-      <c r="D35" s="72"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
       <c r="E35" s="34">
         <v>4</v>
       </c>
@@ -3086,16 +3092,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="33">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B36" s="71" t="s">
+      <c r="B36" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="72"/>
-      <c r="D36" s="72"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
       <c r="E36" s="34">
         <v>2</v>
       </c>
@@ -3103,16 +3109,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="33">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B37" s="77" t="s">
+      <c r="B37" s="80" t="s">
         <v>103</v>
       </c>
-      <c r="C37" s="78"/>
-      <c r="D37" s="78"/>
+      <c r="C37" s="81"/>
+      <c r="D37" s="81"/>
       <c r="E37" s="34">
         <v>6</v>
       </c>
@@ -3120,16 +3126,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="36">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B38" s="73" t="s">
+      <c r="B38" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="C38" s="74"/>
-      <c r="D38" s="74"/>
+      <c r="C38" s="77"/>
+      <c r="D38" s="77"/>
       <c r="E38" s="37">
         <v>2</v>
       </c>
@@ -3137,16 +3143,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="36">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B39" s="73" t="s">
+      <c r="B39" s="76" t="s">
         <v>116</v>
       </c>
-      <c r="C39" s="74"/>
-      <c r="D39" s="74"/>
+      <c r="C39" s="77"/>
+      <c r="D39" s="77"/>
       <c r="E39" s="37">
         <v>10</v>
       </c>
@@ -3154,16 +3160,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="36">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="76" t="s">
         <v>117</v>
       </c>
-      <c r="C40" s="74"/>
-      <c r="D40" s="74"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="77"/>
       <c r="E40" s="37">
         <v>6</v>
       </c>
@@ -3171,16 +3177,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="36">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B41" s="73" t="s">
+      <c r="B41" s="76" t="s">
         <v>118</v>
       </c>
-      <c r="C41" s="74"/>
-      <c r="D41" s="74"/>
+      <c r="C41" s="77"/>
+      <c r="D41" s="77"/>
       <c r="E41" s="37">
         <v>4</v>
       </c>
@@ -3188,16 +3194,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="36">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B42" s="73" t="s">
+      <c r="B42" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="C42" s="74"/>
-      <c r="D42" s="74"/>
+      <c r="C42" s="77"/>
+      <c r="D42" s="77"/>
       <c r="E42" s="37">
         <v>4</v>
       </c>
@@ -3205,16 +3211,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="36">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B43" s="73" t="s">
+      <c r="B43" s="76" t="s">
         <v>120</v>
       </c>
-      <c r="C43" s="74"/>
-      <c r="D43" s="74"/>
+      <c r="C43" s="77"/>
+      <c r="D43" s="77"/>
       <c r="E43" s="37">
         <v>2</v>
       </c>
@@ -3222,16 +3228,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="36">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="78" t="s">
         <v>103</v>
       </c>
-      <c r="C44" s="76"/>
-      <c r="D44" s="76"/>
+      <c r="C44" s="79"/>
+      <c r="D44" s="79"/>
       <c r="E44" s="37">
         <v>6</v>
       </c>
@@ -3248,15 +3254,15 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" s="33">
         <v>64</v>
       </c>
-      <c r="B45" s="71" t="s">
+      <c r="B45" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C45" s="72"/>
-      <c r="D45" s="72"/>
+      <c r="C45" s="75"/>
+      <c r="D45" s="75"/>
       <c r="E45" s="34">
         <v>2</v>
       </c>
@@ -3273,13 +3279,13 @@
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A46" s="33"/>
-      <c r="B46" s="77" t="s">
+      <c r="B46" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C46" s="78"/>
-      <c r="D46" s="78"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="81"/>
       <c r="E46" s="34"/>
       <c r="F46" s="35"/>
       <c r="L46" s="47" t="s">
@@ -3292,16 +3298,16 @@
         <v>154</v>
       </c>
     </row>
-    <row r="47" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A47" s="36">
         <f>A45+32</f>
         <v>96</v>
       </c>
-      <c r="B47" s="73" t="s">
+      <c r="B47" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C47" s="74"/>
-      <c r="D47" s="74"/>
+      <c r="C47" s="77"/>
+      <c r="D47" s="77"/>
       <c r="E47" s="37">
         <v>2</v>
       </c>
@@ -3318,13 +3324,13 @@
         <v>153</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A48" s="36"/>
-      <c r="B48" s="75" t="s">
+      <c r="B48" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C48" s="76"/>
-      <c r="D48" s="76"/>
+      <c r="C48" s="79"/>
+      <c r="D48" s="79"/>
       <c r="E48" s="37"/>
       <c r="F48" s="38"/>
       <c r="L48" s="47" t="s">
@@ -3337,16 +3343,16 @@
         <v>152</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A49" s="33">
         <f>A47+32</f>
         <v>128</v>
       </c>
-      <c r="B49" s="71" t="s">
+      <c r="B49" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C49" s="72"/>
-      <c r="D49" s="72"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="75"/>
       <c r="E49" s="34">
         <v>2</v>
       </c>
@@ -3363,13 +3369,13 @@
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A50" s="33"/>
-      <c r="B50" s="77" t="s">
+      <c r="B50" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C50" s="78"/>
-      <c r="D50" s="78"/>
+      <c r="C50" s="81"/>
+      <c r="D50" s="81"/>
       <c r="E50" s="34"/>
       <c r="F50" s="35"/>
       <c r="L50" s="47" t="s">
@@ -3382,16 +3388,16 @@
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A51" s="36">
         <f>A49+32</f>
         <v>160</v>
       </c>
-      <c r="B51" s="73" t="s">
+      <c r="B51" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
+      <c r="C51" s="77"/>
+      <c r="D51" s="77"/>
       <c r="E51" s="37">
         <v>2</v>
       </c>
@@ -3408,13 +3414,13 @@
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="36"/>
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C52" s="76"/>
-      <c r="D52" s="76"/>
+      <c r="C52" s="79"/>
+      <c r="D52" s="79"/>
       <c r="E52" s="37"/>
       <c r="F52" s="38"/>
       <c r="L52" s="47" t="s">
@@ -3427,16 +3433,16 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="33">
         <f>A51+32</f>
         <v>192</v>
       </c>
-      <c r="B53" s="71" t="s">
+      <c r="B53" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C53" s="72"/>
-      <c r="D53" s="72"/>
+      <c r="C53" s="75"/>
+      <c r="D53" s="75"/>
       <c r="E53" s="34">
         <v>2</v>
       </c>
@@ -3453,13 +3459,13 @@
         <v>147</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A54" s="33"/>
-      <c r="B54" s="77" t="s">
+      <c r="B54" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="81"/>
       <c r="E54" s="34"/>
       <c r="F54" s="35"/>
       <c r="L54" s="47" t="s">
@@ -3472,16 +3478,16 @@
         <v>146</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A55" s="36">
         <f>A53+32</f>
         <v>224</v>
       </c>
-      <c r="B55" s="73" t="s">
+      <c r="B55" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C55" s="74"/>
-      <c r="D55" s="74"/>
+      <c r="C55" s="77"/>
+      <c r="D55" s="77"/>
       <c r="E55" s="37">
         <v>2</v>
       </c>
@@ -3498,13 +3504,13 @@
         <v>145</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A56" s="36"/>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C56" s="76"/>
-      <c r="D56" s="76"/>
+      <c r="C56" s="79"/>
+      <c r="D56" s="79"/>
       <c r="E56" s="37"/>
       <c r="F56" s="38"/>
       <c r="L56" s="47" t="s">
@@ -3517,16 +3523,16 @@
         <v>144</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A57" s="33">
         <f>A55+32</f>
         <v>256</v>
       </c>
-      <c r="B57" s="71" t="s">
+      <c r="B57" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C57" s="72"/>
-      <c r="D57" s="72"/>
+      <c r="C57" s="75"/>
+      <c r="D57" s="75"/>
       <c r="E57" s="34">
         <v>2</v>
       </c>
@@ -3543,13 +3549,13 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A58" s="33"/>
-      <c r="B58" s="77" t="s">
+      <c r="B58" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="78"/>
-      <c r="D58" s="78"/>
+      <c r="C58" s="81"/>
+      <c r="D58" s="81"/>
       <c r="E58" s="34"/>
       <c r="F58" s="35"/>
       <c r="L58" s="47" t="s">
@@ -3562,16 +3568,16 @@
         <v>142</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A59" s="36">
         <f>A57+32</f>
         <v>288</v>
       </c>
-      <c r="B59" s="73" t="s">
+      <c r="B59" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C59" s="74"/>
-      <c r="D59" s="74"/>
+      <c r="C59" s="77"/>
+      <c r="D59" s="77"/>
       <c r="E59" s="37">
         <v>2</v>
       </c>
@@ -3588,13 +3594,13 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="210" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A60" s="36"/>
-      <c r="B60" s="75" t="s">
+      <c r="B60" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C60" s="76"/>
-      <c r="D60" s="76"/>
+      <c r="C60" s="79"/>
+      <c r="D60" s="79"/>
       <c r="E60" s="37"/>
       <c r="F60" s="38"/>
       <c r="L60" s="47" t="s">
@@ -3607,16 +3613,16 @@
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A61" s="33">
         <f>A59+32</f>
         <v>320</v>
       </c>
-      <c r="B61" s="71" t="s">
+      <c r="B61" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C61" s="72"/>
-      <c r="D61" s="72"/>
+      <c r="C61" s="75"/>
+      <c r="D61" s="75"/>
       <c r="E61" s="34">
         <v>2</v>
       </c>
@@ -3633,13 +3639,13 @@
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="33"/>
-      <c r="B62" s="77" t="s">
+      <c r="B62" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C62" s="78"/>
-      <c r="D62" s="78"/>
+      <c r="C62" s="81"/>
+      <c r="D62" s="81"/>
       <c r="E62" s="34"/>
       <c r="F62" s="35"/>
       <c r="L62" s="47" t="s">
@@ -3652,16 +3658,16 @@
         <v>136</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="36">
         <f>A61+32</f>
         <v>352</v>
       </c>
-      <c r="B63" s="73" t="s">
+      <c r="B63" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C63" s="74"/>
-      <c r="D63" s="74"/>
+      <c r="C63" s="77"/>
+      <c r="D63" s="77"/>
       <c r="E63" s="37">
         <v>2</v>
       </c>
@@ -3678,13 +3684,13 @@
         <v>135</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="36"/>
-      <c r="B64" s="75" t="s">
+      <c r="B64" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C64" s="76"/>
-      <c r="D64" s="76"/>
+      <c r="C64" s="79"/>
+      <c r="D64" s="79"/>
       <c r="E64" s="37"/>
       <c r="F64" s="38"/>
       <c r="L64" s="47" t="s">
@@ -3697,16 +3703,16 @@
         <v>134</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A65" s="33">
         <f>A63+32</f>
         <v>384</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C65" s="72"/>
-      <c r="D65" s="72"/>
+      <c r="C65" s="75"/>
+      <c r="D65" s="75"/>
       <c r="E65" s="34">
         <v>2</v>
       </c>
@@ -3723,26 +3729,26 @@
         <v>132</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A66" s="33"/>
-      <c r="B66" s="77" t="s">
+      <c r="B66" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C66" s="78"/>
-      <c r="D66" s="78"/>
+      <c r="C66" s="81"/>
+      <c r="D66" s="81"/>
       <c r="E66" s="34"/>
       <c r="F66" s="35"/>
     </row>
-    <row r="67" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="36">
         <f>A65+32</f>
         <v>416</v>
       </c>
-      <c r="B67" s="73" t="s">
+      <c r="B67" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C67" s="74"/>
-      <c r="D67" s="74"/>
+      <c r="C67" s="77"/>
+      <c r="D67" s="77"/>
       <c r="E67" s="37">
         <v>2</v>
       </c>
@@ -3759,13 +3765,13 @@
         <v>129</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A68" s="36"/>
-      <c r="B68" s="75" t="s">
+      <c r="B68" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C68" s="76"/>
-      <c r="D68" s="76"/>
+      <c r="C68" s="79"/>
+      <c r="D68" s="79"/>
       <c r="E68" s="37"/>
       <c r="F68" s="38"/>
       <c r="L68" s="50" t="s">
@@ -3778,16 +3784,16 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="33">
         <f>A67+32</f>
         <v>448</v>
       </c>
-      <c r="B69" s="71" t="s">
+      <c r="B69" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C69" s="72"/>
-      <c r="D69" s="72"/>
+      <c r="C69" s="75"/>
+      <c r="D69" s="75"/>
       <c r="E69" s="34">
         <v>2</v>
       </c>
@@ -3804,13 +3810,13 @@
         <v>125</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="33"/>
-      <c r="B70" s="77" t="s">
+      <c r="B70" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C70" s="78"/>
-      <c r="D70" s="78"/>
+      <c r="C70" s="81"/>
+      <c r="D70" s="81"/>
       <c r="E70" s="34"/>
       <c r="F70" s="35"/>
       <c r="L70" s="44" t="s">
@@ -3823,16 +3829,16 @@
         <v>123</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="36">
         <f>A69+32</f>
         <v>480</v>
       </c>
-      <c r="B71" s="73" t="s">
+      <c r="B71" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C71" s="74"/>
-      <c r="D71" s="74"/>
+      <c r="C71" s="77"/>
+      <c r="D71" s="77"/>
       <c r="E71" s="37">
         <v>2</v>
       </c>
@@ -3840,26 +3846,26 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="36"/>
-      <c r="B72" s="75" t="s">
+      <c r="B72" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C72" s="76"/>
-      <c r="D72" s="76"/>
+      <c r="C72" s="79"/>
+      <c r="D72" s="79"/>
       <c r="E72" s="37"/>
       <c r="F72" s="38"/>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="33">
         <f>A71+32</f>
         <v>512</v>
       </c>
-      <c r="B73" s="71" t="s">
+      <c r="B73" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C73" s="72"/>
-      <c r="D73" s="72"/>
+      <c r="C73" s="75"/>
+      <c r="D73" s="75"/>
       <c r="E73" s="34">
         <v>2</v>
       </c>
@@ -3867,26 +3873,26 @@
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="33"/>
-      <c r="B74" s="77" t="s">
+      <c r="B74" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C74" s="78"/>
-      <c r="D74" s="78"/>
+      <c r="C74" s="81"/>
+      <c r="D74" s="81"/>
       <c r="E74" s="34"/>
       <c r="F74" s="35"/>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="36">
         <f>A73+32</f>
         <v>544</v>
       </c>
-      <c r="B75" s="73" t="s">
+      <c r="B75" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C75" s="74"/>
-      <c r="D75" s="74"/>
+      <c r="C75" s="77"/>
+      <c r="D75" s="77"/>
       <c r="E75" s="37">
         <v>2</v>
       </c>
@@ -3894,26 +3900,26 @@
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="36"/>
-      <c r="B76" s="75" t="s">
+      <c r="B76" s="78" t="s">
         <v>122</v>
       </c>
-      <c r="C76" s="76"/>
-      <c r="D76" s="76"/>
+      <c r="C76" s="79"/>
+      <c r="D76" s="79"/>
       <c r="E76" s="37"/>
       <c r="F76" s="38"/>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="33">
         <f>A75+32</f>
         <v>576</v>
       </c>
-      <c r="B77" s="71" t="s">
+      <c r="B77" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="C77" s="72"/>
-      <c r="D77" s="72"/>
+      <c r="C77" s="75"/>
+      <c r="D77" s="75"/>
       <c r="E77" s="34">
         <v>2</v>
       </c>
@@ -3921,26 +3927,26 @@
         <v>18</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="33"/>
-      <c r="B78" s="77" t="s">
+      <c r="B78" s="80" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="78"/>
-      <c r="D78" s="78"/>
+      <c r="C78" s="81"/>
+      <c r="D78" s="81"/>
       <c r="E78" s="34"/>
       <c r="F78" s="35"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="36">
         <f>A77+32</f>
         <v>608</v>
       </c>
-      <c r="B79" s="73" t="s">
+      <c r="B79" s="76" t="s">
         <v>121</v>
       </c>
-      <c r="C79" s="74"/>
-      <c r="D79" s="74"/>
+      <c r="C79" s="77"/>
+      <c r="D79" s="77"/>
       <c r="E79" s="37">
         <v>2</v>
       </c>
@@ -3948,16 +3954,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A80" s="39">
         <f>A79+26</f>
         <v>634</v>
       </c>
-      <c r="B80" s="79" t="s">
+      <c r="B80" s="82" t="s">
         <v>103</v>
       </c>
-      <c r="C80" s="80"/>
-      <c r="D80" s="80"/>
+      <c r="C80" s="83"/>
+      <c r="D80" s="83"/>
       <c r="E80" s="40">
         <v>6</v>
       </c>
@@ -3965,24 +3971,24 @@
         <v>19</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="84" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="84" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>167</v>
       </c>
-      <c r="B84" s="81" t="s">
+      <c r="B84" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="C84" s="82" t="s">
+      <c r="C84" s="56" t="s">
         <v>159</v>
       </c>
-      <c r="D84" s="82" t="s">
+      <c r="D84" s="56" t="s">
         <v>160</v>
       </c>
-      <c r="E84" s="82" t="s">
+      <c r="E84" s="56" t="s">
         <v>161</v>
       </c>
-      <c r="F84" s="83" t="s">
+      <c r="F84" s="57" t="s">
         <v>162</v>
       </c>
       <c r="G84" s="54"/>
@@ -3991,7 +3997,7 @@
       <c r="J84" s="54"/>
       <c r="K84" s="54"/>
     </row>
-    <row r="85" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B85" s="54"/>
       <c r="C85" s="54"/>
       <c r="D85" s="54"/>
@@ -4005,74 +4011,74 @@
       <c r="J85" s="54"/>
       <c r="K85" s="54"/>
     </row>
-    <row r="86" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>168</v>
       </c>
-      <c r="B86" s="81">
+      <c r="B86" s="55">
         <v>1</v>
       </c>
-      <c r="C86" s="82" t="s">
+      <c r="C86" s="56" t="s">
         <v>163</v>
       </c>
-      <c r="D86" s="82">
+      <c r="D86" s="56">
         <v>2</v>
       </c>
-      <c r="E86" s="82" t="s">
+      <c r="E86" s="56" t="s">
         <v>164</v>
       </c>
-      <c r="F86" s="82">
+      <c r="F86" s="56">
         <v>3</v>
       </c>
-      <c r="G86" s="82" t="s">
+      <c r="G86" s="56" t="s">
         <v>165</v>
       </c>
-      <c r="H86" s="82">
+      <c r="H86" s="56">
         <v>4</v>
       </c>
-      <c r="I86" s="82" t="s">
+      <c r="I86" s="56" t="s">
         <v>166</v>
       </c>
-      <c r="J86" s="82">
+      <c r="J86" s="56">
         <v>5</v>
       </c>
-      <c r="K86" s="83" t="s">
+      <c r="K86" s="57" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="88" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="88" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>168</v>
       </c>
-      <c r="B88" s="81" t="s">
+      <c r="B88" s="55" t="s">
         <v>169</v>
       </c>
-      <c r="C88" s="82" t="s">
+      <c r="C88" s="56" t="s">
         <v>170</v>
       </c>
-      <c r="D88" s="82" t="s">
+      <c r="D88" s="56" t="s">
         <v>171</v>
       </c>
-      <c r="E88" s="82" t="s">
+      <c r="E88" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="F88" s="82" t="s">
+      <c r="F88" s="56" t="s">
         <v>172</v>
       </c>
-      <c r="G88" s="82" t="s">
+      <c r="G88" s="56" t="s">
         <v>176</v>
       </c>
-      <c r="H88" s="82" t="s">
+      <c r="H88" s="56" t="s">
         <v>173</v>
       </c>
-      <c r="I88" s="82" t="s">
+      <c r="I88" s="56" t="s">
         <v>177</v>
       </c>
-      <c r="J88" s="82" t="s">
+      <c r="J88" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="K88" s="83" t="s">
+      <c r="K88" s="57" t="s">
         <v>178</v>
       </c>
     </row>

</xml_diff>